<commit_message>
Get daily reddit data: Tue Jun 11 08:09:43 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_16.xlsx
+++ b/data/2024_06_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C474"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2947 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1dd7vyg</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">90s Press Ons I Made for a party </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gl587hns4w5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1dd7vat</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Got my nails done last night</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p91prhyj4w5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1dd7mec</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Venom by ILNP</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lx0tu8ra1w5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1dd6dw1</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Princess Vibes 💫🩷🩵 inspired by oaklestudio on IG</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd6dw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1dd62kh</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Birthday Nails ❣️</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn4v25h2jv5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1dd4392</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Taking suggestions!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd4392/taking_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1dd4diz</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Quick drying, non-gel polish recs?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd4diz/quick_drying_nongel_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1dd5j1x</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Who has the simply nailogical/moon cat vibes but is gel and as affordable as them? </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd5j1x/who_has_the_simply_nailogicalmoon_cat_vibes_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1dd5b09</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>love my japanese gel nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd5b09</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1dd5au4</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Where can I find the brush she’s using? @heygreatnails</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69vts1t0bv5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1dd4zhf</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Finally tried almond!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd4zhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1dd4j6h</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>First professional French manicure</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zury5a883v5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1dd4ht2</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>be a superstar not only a star</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7ioc4qo2v5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1dd3p0a</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Should I get these fixed?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd3p0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1dd43b2</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Worked with kids, did something very simple this week. </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoo127jxyu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1dd3zhc</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A moment for the fresh set </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6faldwvvxu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1dd391x</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Nailz</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72ace9dyqu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1dd3846</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>OPI Blue Moon Lagoon</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd3846</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1dd331l</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Just your friendly neighborhood bisexual checking in for Pride Month!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd331l</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1dd2uv2</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>My nails for the upcoming Megan thee Stallion concert in HTX</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9vm1pbwcnu5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1dd2rlu</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Have I been going to the wrong nail salons or…?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd2rlu/have_i_been_going_to_the_wrong_nail_salons_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1dd2jh2</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>What’s up with these white lines? Do my nails need moisture?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82prcypdku5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1dd26ax</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye attempt </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q629z61hu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1dd1zyq</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Weak nails normal? </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd1zyq/weak_nails_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1dd1xnp</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>tried a new color ☀️</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dduhy6tteu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1dd1u3i</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Pride Nails! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd1u3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1dd1j27</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Ocean nails for the summer 💙🐟</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pud29k6bu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1dd0mcv</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Best nail polish for natural nails?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd0mcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1dd0ztt</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Advice: Dashing Diva Nail Strengthener Gel Kit</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adcucoab6u5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1dd1aju</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>New nail day 🍄🌱🐞✨</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd1aju</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1dd13yu</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Pride Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd13yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1dd0yo2</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Janet Jackson Nails </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd0yo2/janet_jackson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1dd0r0g</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Nail Bipolar</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd0r0g/nail_bipolar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1dd0e11</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my instructors nails today! </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd0e11</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1dczt7d</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Summer florals!!</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl1xrzv0wt5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1dczx2w</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Help me get through the next 3 weeks 🤣</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dczx2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1dczt45</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Rick and Morty #rickandmorty</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dczt45</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1dczqjd</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My latest set 💛</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dczqjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1dczov2</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Are Massage Chairs annoying?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dczov2/are_massage_chairs_annoying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1dczdpa</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Ilnp combo</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dczdpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1dczci6</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Nail Tips</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dczci6/nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1dczbap</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Need your opinions</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dczbap/need_your_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1dcyxu7</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I just got acrylic nails and I’m sooo exited I love them sm</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcyxu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1dcyx29</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regular manicure question </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcyx29/regular_manicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1dcysf6</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Mailnails</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpkr1h3unt5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1dcyqsn</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Baby shower nails! Mixed feelings about the paw print</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rsu8n6hnt5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1dcxxbn</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Is this dip or acrylics?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc5xwoh4ht5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1dcxtng</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Please help me find a neutral polish!?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfymuyubgt5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1dcxr1b</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wanted to try something new </t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsv0oenrft5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1dcx7gz</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Hypoallergenic korean/japanese gel brands?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcx7gz/hypoallergenic_koreanjapanese_gel_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1dcxc4y</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>gel x or normal gel?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcxc4y/gel_x_or_normal_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1dcxlmh</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling extra girly with these nails! Done by myself </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kwiigulet5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1dcxby3</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>French perfect⚪️☑️</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcxby3</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1dcwxhd</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Pride Month 🌈 featuring kitty in cone of shame :(</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcwxhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1dcwsfw</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>BIAB on natural nails w/ gold stickers (ignore the cuticles!)</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi97c68m8t5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1dcwpof</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Biogel vs BIAB vs Builder Gel</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcwpof/biogel_vs_biab_vs_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1dcwo0z</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>I hold builder gel help these nails?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcwo0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1dcwg7k</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Brought my own dried flowers to my nail tech and asked for "wildflower nails." What's the verdict?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcwg7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1dcwei8</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>My nails are ready for this summer (by myself) ☀️</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ca5coqvr5t5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1dcwdi4</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Which nail shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcwdi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1dcw7x6</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Scale/Seashell Cat eye</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcw7x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1dcvosu</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>I'm in love. Used a filter only because it's closer to the actual color, camera wasn't picking it up. I feel like a 90s sunset!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nt2jvlrk0t5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1dcud0w</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>I can’t get over these nails !</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmt3vk16rs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1dcur4k</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Some rhinestones to start the week💎</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iw38sdj0us5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1dculbn</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Halloween cats eye throwback</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbljtkvuss5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1dcujkx</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Nails right after being done. Love the color, but does it look like they are grown out already?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb3i7x5iss5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1dcudux</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Lucky charm 🍀</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xu488ebrs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1dcu89e</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Am I being too picky or these are not worth the €40 I've paid?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a4rfzg7qs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1dcu7f1</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Red French tip and some glitter featuring my lil turtle friend</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebgk4fc1qs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1dcu78d</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Esculpidas en acrílico! Que les parece?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc1uyw30qs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1dcu2ic</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Freehand porcelain press ons</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/amv8w632ps5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1dcu10f</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Miren esto 😍</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv9yzrlros5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1dcu0d2</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Les gusta estos clore?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a3aooumos5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1dctzws</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Good!?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cko2rpvjos5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1dctzvz</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Letting my nails grow 🤩</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfe85uqjos5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1dctzhn</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uñas Xl! </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0dsk6kgos5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1dctwc0</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Finally decided to do my nails after a while</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dctwc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1dctjfy</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>What do you think of the design?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv73cg8als5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1dcta8c</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Latest set 💅🏼🖤🏁❤️‍🔥⛓️</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11nuejwijs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1dcta0r</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcta0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1dct5hy</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Always let me tech freestyle because she gets me🫶🏼</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dct5hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1dct58u</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Clean girl vibes</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dct58u</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1dct3hj</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Man nails art first Time (by my wife)</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dct3hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1dct0oz</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy pride. Bet you can't guess which hand is my dominant </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dct0oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1dcssby</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Graffiti nails🔥😈💔</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcssby</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1dcsn7x</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Trying something different</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iskrddszes5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1dcshs9</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Been doing my own nails for years ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scuntr8vds5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1dcsbt5</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Sister, who is a nail tech, doesn't do my nails.</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcsbt5/sister_who_is_a_nail_tech_doesnt_do_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1dcsb1b</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>so kawaii!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xshfs47hcs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1dcs6gu</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Experimented with 3D builder gel and I’m obsessed with the results! </t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owlozbukbs5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1dcs379</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>I did bug nails!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcs379</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1dcrzc7</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So...I tried my best to do French tips at home with press on nails lol </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwmotrh6as5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1dcmznr</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails Recommendation </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcmznr/nails_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1dcri12</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Pride Nails 2.0</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcri12</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1dcrjbw</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I’m in love with my new nails.</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/587esqjx6s5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1dcnmiw</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Do you think that square nails would fit me?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcnmiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1dchc8l</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Chemical etcher</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dchc8l/chemical_etcher/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1dcdblv</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Allergic to Beetles gel polish</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcdblv/allergic_to_beetles_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1dcqxbp</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>what is hard gel extenstion using forms</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dcqxbp/what_is_hard_gel_extenstion_using_forms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1dcovqc</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Lime Green for Festival Szn 🟩</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ok0qiignr5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1dd8grz</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Trying to manifest some warmer weather with coral red</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuh65lu7cw5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1dd8fau</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Looking for a tool</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dd8fau/looking_for_a_tool/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1dd7egb</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Magnetic Jelly Watermelons🍉✨</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oyt8f0jnyv5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1dd6fa4</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Thermals &amp; photochromic polish</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dd6fa4/thermals_photochromic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1dd64sw</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Freshly Cut</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x4g66crjv5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1dd5p5e</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Cirque Colors Jade Jelly &amp; chrome powder 🧚🏼✨</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pg3f9p4fv5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1dd5ebd</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>I may have a problem…</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7rw8ik1cv5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1dd58ch</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple Holo Shimmer Perfection </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd58ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1dd4e5k</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Officially a thermal convert, but now I have questions and need recommendations. Halp!!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kprury6u1v5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1dd38e1</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>OPI Blue Moon Lagoon</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd38e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1dd34iy</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Swatch request - LynB Happy Haunting vs Cirque Wild Berry West</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dd34iy/swatch_request_lynb_happy_haunting_vs_cirque_wild/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1dd30ux</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Call me obsessed ✨</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd30ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1dd2wvs</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Light up glitter</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0tplvivnu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1dd1efs</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Mostly Mooncat Birthday Skittle</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd1efs</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1dd0zd7</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Pride Nails 🌈 (plus two hand photo hack)</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd0zd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1dd0bv6</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Death Valley Nails- Dreamsickle! </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd0bv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1dd00ic</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Are there iridiscent toppers that are also magnetic and NOT gel based?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dd00ic/are_there_iridiscent_toppers_that_are_also/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1dczozk</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Builder gel lifting at free edge</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dczozk/builder_gel_lifting_at_free_edge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1dczmbf</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Never thought I’d enjoy wearing blue so much</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4xplrseut5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1dczln0</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Kiss ImPRESS Size Exchange?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dczln0/kiss_impress_size_exchange/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1dczfiq</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Let’s use allll the colors</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dczfiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1dcydqu</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Thickest hardest topcoat?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcydqu/thickest_hardest_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1dcxub6</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Neutral nail polish help please!</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lmayo7hgt5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1dcxlbs</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Chicago Lacqueristas</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcxlbs/chicago_lacqueristas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1dcxc8y</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Hypoallergenic korean/japanese brands?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcxc8y/hypoallergenic_koreanjapanese_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1dcx9vn</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Unpopular opinion: white crellies</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcx9vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1dcvgo2</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Looking for a specific kind of topper</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcvgo2/looking_for_a_specific_kind_of_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1dcvacz</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>What's causing my polish to look cloudy after a few days?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcvacz</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1dcv6xn</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Pride nails 🏳️‍🌈💅 (really struggle w/showcasing both hands, pls lmk which format you like!)</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcv6xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1dcurhw</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Flower Child 🌸✨</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcurhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1dctfx6</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>BCB Lacquer</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dctfx6/bcb_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1dct3x1</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Blue Nails with Gel Top Coat</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dct3x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1dcr8cu</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Wipeout from Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/128rq7xp4s5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1dcqu3r</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Which brands ALWAYS come with a wide rounded brush?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03m1vsev1s5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1dcqgrf</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Proudly representing my sexuality (demisexual) with the asexual flag colours (I'll probably be wearing these for pride parade in August)</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/le1bzbpwyr5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1dcqbco</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to cry. Why are my nails like this? :( my nails aren’t a pie crust so why so flaky </t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcqbco</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1dcq1hw</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Flower child</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcq1hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1dcq0e5</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Flat flared nails</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcq0e5/flat_flared_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1dcpzfd</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Photos don’t do it justice</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcpzfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1dcpi4k</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>What are the best gel polishes?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcpi4k/what_are_the_best_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1dcpcb5</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Picasso Moth 🖼️</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcpcb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1dcp8r0</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Tendresse by Penelope Luz</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcp8r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1dcp27c</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I Am With My Friends</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcp27c</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1dcowdn</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>ISO baby blue magnetic polish</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcowdn/iso_baby_blue_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1dcohgl</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Polishes that are similar to Femme Fatale | I Hate Mondays? (PPU)</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb6lom8mkr5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1dcnwkb</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kiwi nails </t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knir35w8gr5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1dcm96a</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Fluttering in the sunlight</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcm96a</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1dcllhu</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer blues </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y7z6uadyq5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1dckqr4</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>💙💜Bi Pride Flag💜🩷</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dckqr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1dcjizp</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Do any of you know, when Nailland and Hypnotic Polish usually do sales?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcjizp/do_any_of_you_know_when_nailland_and_hypnotic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1dcj1ru</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily de Molly - Never Found It &amp; The Same Path </t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcj1ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1dcih3d</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So pleased with how these came out! </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ja6kn5v3q5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1dchwqr</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dchwqr/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1dchwqg</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dchwqg/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1dch9m8</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat fake halo &amp; leaf nail sticker </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dch9m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1dd50tp</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phtxqfha8v5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1dd269c</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone asked me to do Shark Week themed nails. </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpcfi8s0hu5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1dd118o</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Pride Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd118o</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1dcxxum</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Bob esponja 🧽</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcxxum</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1dcxv82</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>I've been in this community for a while, and many of you know me . I've shared my designs, receiving mixed feedback. A fan recently asked for custom hand-painted nail art. As an art graduate, I created a cat-themed set for her .She asked to feature it in my shop under her name, which I think is cool</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcxv82</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1dcxh3o</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>When press ons fit perfectly 😍</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcxh3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1dcw5o6</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Scale/seashell nails</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcw5o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1dcu9vw</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Finding good Cat Eye UV polish</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dcu9vw/finding_good_cat_eye_uv_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1dcu36o</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Freehand porcelain press ons</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21gv5027ps5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1dcqhg3</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>More Pride Nails</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/589juoeezr5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1dcq0u6</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Delicate nail art for my mom</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcq0u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1dcpq6b</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Dare to make eye contact with this? 👀💅</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7ef3w57rtr5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1dcnxyp</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Tips for french nailtip</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dcnxyp/tips_for_french_nailtip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1dcn7gk</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Hey guys, how are you? I dedicate myself to doing nails, dyeing hairstyles, etc. Here I show you a little of my work🥰 I accept any constructive criticism🙌</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhd7o6l4br5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1dcm8bt</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Que piensan de estas uñas ?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrfwylai3r5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1dclx7o</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trabajo de uñas de mi alumna como principiante! </t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd0jsuw11r5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1dcj599</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>🛸GALAKTIKA🛸by yours truly 🖤</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcj599</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1dcihn6</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainbow nails! </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueylllz14q5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun 12 08:08:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_16.xlsx
+++ b/data/2024_06_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C474"/>
+  <dimension ref="A1:C644"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8491,6 +8491,2896 @@
         </is>
       </c>
     </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1de0ds9</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I hated my old colour (update) </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4737oimp936d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1de0d3g</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>what nails would look best with dark green velvet and gold?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de0d3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1de0018</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Nude Nails! 🤩 I so happy with how they came out!!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de0018</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1ddzorj</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Simple manicure ⭐️💕</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yleo8z8136d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1ddzjqz</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>my birthday nails! 🎀</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddzjqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1ddxsgw</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I trick my sister into getting her nails done for her proposal? </t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddxsgw/how_do_i_trick_my_sister_into_getting_her_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1ddyvo9</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Nails pt.2 (more pics)</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddyvo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1ddykh0</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>What can I do better?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddykh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1ddyg1k</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Hopefully these ones last!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddyg1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1ddybh6</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Boring girl vibes</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddybh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1ddy3tb</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Going through my stash</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddy3tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1ddy2gl</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>What shape would best fit my nails/hands?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddy2gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ddxpbp</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Gel manicure lifting 6 days</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddxpbp/gel_manicure_lifting_6_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ddxege</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>How do i make long acrylic nails last as long as possible?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbvocja1c26d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ddvvs4</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice please? </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddvvs4/advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ddwvvu</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I have put the cat eye line like this or going opposite ways? </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvgmha6t626d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ddwew4</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>I'm in love with being a basic white girl 💓</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1oj3ix5226d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ddw76p</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOO!🐮 </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddw76p</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ddw6iw</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Is there an option for my nails that’s an “in between” of gel polish and dip powder?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddw6iw/is_there_an_option_for_my_nails_thats_an_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ddvzsb</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Fresh manicure</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/754n3rv3y16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ddvgly</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Breaking nail biting habit of 30ish years</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddvgly</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ddvkoh</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Hey! It’s my first time posting. I just want to share my pride nails! ☀️</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hnozxs4u16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ddvcfz</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>why is there a small nail under my real nail?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddvcfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ddv770</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">finally seeing improvements </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu8q19sqq16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1dduzw5</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>First time trying purple</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh6mytauo16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1dduq50</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Do you think the color gray looks good?</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkd7x2jbm16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ddupqu</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wife recently started doing her own nails. I don't know much about the hobby but I think they look amazing. </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddupqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1dduj32</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Good for 4 weeks?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc0t9qlik16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1dduh44</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love ombre! </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trax04lzj16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1dduh2n</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍒love my nail tech </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbfhx26zj16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1dduc08</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Need a fill and can’t get an appt</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dduc08/need_a_fill_and_cant_get_an_appt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1ddu8kp</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>In honor of Pride month.</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo7j62wuh16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1ddu6h7</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>2 days shy of 4 weeks!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddu6h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1ddu41n</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Bleached Neon Love 💛</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddu41n</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ddsjrf</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>How long does it take for the Proximal Nail Fold to grow back, and does it scar?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpnxquvw216d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1ddtygx</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>birthday set for my birthday trip to  Greece! 🤩♊️</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5h5j54m8f16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1ddtwko</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>half cover tips + Bissu glitter + hard gel</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dafin9tqe16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1ddtrf7</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>I don’t even wanna tell you guys how long this took 😅 BUT my cuticle work is getting a lot better and I love how these turned out!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1dau9fgd16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1ddtot1</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Ahhh, summer nails 💗</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0tusaatc16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ddtns5</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Gel overlay and cuticle oil have made my nailbed so much longer, finally!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c8xvwvkc16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ddtmc4</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksczb3x6c16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ddtkal</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make press on nails look natural </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddtkal/how_to_make_press_on_nails_look_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ddsz5l</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Acrylic girls… how to remove safely?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh8wzadm616d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ddswma</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Chapelle Roan’s nails for Gov Ball 😍😍😍😍</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddswma</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ddrzeg</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>My GelX suddenly don’t stay on?! *process in body</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddrzeg/my_gelx_suddenly_dont_stay_on_process_in_body/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1dds9l0</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>my first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8mrsgmi016d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1dds6ig</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>First time using gel uv light</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hklftb8tz06d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1dds690</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>First time working with white acrylic</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dds690</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1ddrri7</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Geometric French Press Ons</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddrri7</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1ddr97o</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Scooby dooby doo!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofs6ht36s06d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1ddrbeu</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to start growing my nails again after suffering from my last breakage Nov. ‘23. 1 month in &amp; so far so good. I maintain, shape &amp; paint them myself so don’t expect professional pics here 😂  Pics 1-3 are my old set. Pics 4-5 are my current set. </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddrbeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ddqnc9</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Finally tried stick-ons 💅🏾</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddqnc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1ddoziw</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Best red recommendations</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddoziw/best_red_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1ddowhs</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>What’s wrong with them?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddowhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1ddpmly</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>I love pink nails 💗</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohm7l7npf06d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1ddpkwy</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Chipping polish</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddpkwy/chipping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1ddpdx1</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Any tips on how to get deals on professional brands or find quality dupes? For example: Sweetie Nail Supply</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddpdx1/any_tips_on_how_to_get_deals_on_professional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1ddp8my</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>First time getting tortoise shell and I feel soooo elegant 🤎</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddp8my</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ddp3le</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pride nails </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9n05ihsb06d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ddp03a</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried 3D nail art for the first time! </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddp03a</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ddo1mr</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>NOT MY WORK (Upset)</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddo1mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ddnpuc</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>First DIY set ever!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddnpuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ddnnrz</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Going to a wedding this weekend</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13e180a9106d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ddn6by</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>painted a set of pressons</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddn6by</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1ddmka1</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skin peeling under a singular fingernail </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddmka1/skin_peeling_under_a_singular_fingernail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1ddma4d</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Nails are my favorite accessory! 💅🏾</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddma4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1ddljv3</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail care essentials </t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddljv3/nail_care_essentials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ddl89k</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Structure gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf0437sljz5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1ddl7xz</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>First time to try red french tips 💅🏻</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy5bcubjjz5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1ddl7g3</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Chrome tips</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddl7g3</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1ddkyq8</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Spider-Man Nails</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij7tlwsphz5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1ddkx92</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>How can I make my gels last longer?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddkx92/how_can_i_make_my_gels_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1ddkdth</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Why are the bases of the tips of my nails translucent?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddkdth</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1ddkrxd</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Some Cherry Blossom 3D art 🌸</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du5grq3egz5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1dde4jn</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Chronic nail biter…. Need help</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dde4jn/chronic_nail_biter_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ddddcz</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>My nail beds cracked - can’t find advice</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddddcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1ddkhe5</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Just a bit of sparkle</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfmvx15bez5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1dd94j6</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need help. My nail is killing me. </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd94j6/i_need_help_my_nail_is_killing_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1ddked4</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Is this bad?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddked4</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1dd00g7</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Rant</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dd00g7/rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1ddk4m6</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did my besties nails! Can you tell which ones are gel x? </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19n7b1yqbz5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1ddk466</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which of these nudes suits me best? </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddk466</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1ddjluq</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for beginner </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ddjluq/advice_for_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ddjlot</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>something colorful 💅🏻</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v685h2nq7z5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ddjkuz</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Tell me your opinions</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddjkuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1ddjjga</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French tip varnish that DOESN'T look like corrector fluid? </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyu663wa7z5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1dd8252</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>I feel like the baddest bitch ever with red claws</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dd8252</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1ddjedl</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve worn press on nails for at least a year and the state of my nails are becoming quite bad. What can I do to make them healthy again? I also wondered what can happen if I continue to wear the nails? Thanks. </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agnrcp2a6z5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1ddiymt</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I was about ready to paint my nails and then one of them broke from playing a video game…</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjh9bdr43z5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1ddimv9</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Matcha jelly nails 🍵</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iw7l7jjp0z5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1ddiheo</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Got my Nails Rounded Squared after 3 years of getting Almond.</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7k3kvmkzy5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ddid00</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>my fav set yet!!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9ucvonnyy5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ddhrv3</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Couldn’t decide which shade I liked more so I chose both 💙</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ml4m3zv8uy5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ddhowv</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>First time getting tips and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddhowv</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ddhmp2</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>fresh mid length french tip stilettos. My nail tech did a good job 👏🏻</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmn89vv7ty5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ddhchf</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Ocean opal is my favorite jewelry and I am looking for a nail color/design idea that looks similar? Anyone have any ideas??🩵</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hc2c3kl2ry5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ddgt4y</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Uñas en un tono muy delicado! 🌸</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddgt4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ddgpo3</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>i’ve missed the long stilettos!!</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcest3pdmy5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ddgp1v</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Party nails to kick off summer 🍭</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bosa9069my5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ddgmr2</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>DIY designs on my own nails, ty for the feedback on Sundays post on narrowing down the designs.</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5ztb1fxply5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ddzwo3</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Nude Nails!🤩 ONE of my favorite colors, I personally love these types of colored polishes.</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddzwo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ddxtpp</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Dupe for Nina Ultra Pro Fuschia Rage</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqox60zag26d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ddwutx</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>When you’re moving and pack your polish remover and clips too soon, you have to make do</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o30pordi626d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ddvxzk</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Know a nail color like this?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs39pd0nx16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ddo0b3</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Mooncat Mercury Tears shift</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjzndl6q306d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ddvabp</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Groovy 🌼</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddvabp</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1ddjlov</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Dark Red</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddjlov</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1ddhzl9</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>My EDM haul</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwcot6vsvy5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1dduhag</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Nail scales</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dduhag</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ddu2jr</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Bleached Neon Love 💛</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddu2jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ddu0rc</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Nailtiques formula 2 from CVS</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddu0rc/nailtiques_formula_2_from_cvs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1ddtykq</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Shifty rainbow-y nails for pride</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddtykq</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ddtwgd</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>pandemonium is so pigmented!!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddtwgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ddtg40</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Latest Holiday Set!</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddtg40</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ddsupj</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Stamps for short nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddsupj/stamps_for_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ddssdl</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Anybody else freaking out over Sassy Sauce A Pain In The Asteroid?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddssdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ddss0r</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Anybody else freaking out over Sassy Sauce A Pain In The Asteroid?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddss0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1ddrqra</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Can someone help me identify these colors?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4q34h7bw06d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ddr8v7</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Great nail polish remover I can find in canada?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddr8v7/great_nail_polish_remover_i_can_find_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ddqeba</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>What polish will give me nails like these?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddqeba</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1ddpfe6</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Any tips on how to get deals on professional brands or find quality dupes? For example: Sweetie Nail Supply</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddpfe6/any_tips_on_how_to_get_deals_on_professional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ddoxap</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does blue cross cuticule remover make my nail peel? </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddoxap/why_does_blue_cross_cuticule_remover_make_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ddouye</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Blue and yellow - HELLO</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/h3bobwC.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ddoovm</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Professional this time </t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddoovm</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ddo0gq</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>These colors yalls..</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddo0gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1ddnpmw</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I'm going through a really hard time right now &amp; didn't have the energy to do a perfect job or clean them up immaculately. But I really love my night sky nails 🌌 can't stop admiring them!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddnpmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ddngrd</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Does anyone else change colors multiple times/week? Is this a bad idea?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddngrd/does_anyone_else_change_colors_multiple_timesweek/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ddmvmu</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>This Sub made me buy it..</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddmvmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1ddl8pt</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Ilnp combo</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddl8pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1ddl7g0</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie shrinkage </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddl7g0/essie_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1ddl6pb</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>If you do gel nails at home…</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddl6pb/if_you_do_gel_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ddklqn</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Monarch - Truth or Dare</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddklqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1ddkkxu</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Has anyone had their old nail thicker than their fresh growth after removing gel polish?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddkkxu/has_anyone_had_their_old_nail_thicker_than_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1ddjk9c</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Gotta say, I’m pretty happy with how this Pride gradient turned out. 😌🏳️‍🌈🌈</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddjk9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ddi9xi</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>ILNP Funhouse</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wk9yni0yy5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ddi7xt</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Night Owl Light Dragon &amp; Kathleen &amp; Co Butterfly Nebula</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddi7xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ddi2nn</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Recent nail lüks</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddi2nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ddhw6r</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Apparition 👻</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eqvn59oouy5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1ddhink</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Named polish request?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddhink/named_polish_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1ddh45j</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce Hexcellent </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddh45j</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1ddgoio</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Trans Flag: Pride Flags for Pride</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddgoio</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ddga6p</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Ty everyone for feedback here is the final design on my nails!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6nvphn05jy5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1ddf5xg</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Cajun shrimp + OPI Glazed N’ Amused  </t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc0hzscuay5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ddenpa</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>🖤🩶🏳️‍🌈Ace Pride🏳️‍🌈🤍💜</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddenpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ddek94</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Nail polish safety - freaking myself out and need to be talked down</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ddek94/nail_polish_safety_freaking_myself_out_and_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ddc2lf</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>First time skittle-r. Happy Pride 🌈✨</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddc2lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ddan3a</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer - Ethereal Creature 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5if44jv34x5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1dd0nxa</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Gone fishing? MC+HT combo</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jnv4lzb3u5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1dcwhne</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Airbrush</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dcwhne/airbrush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1dcw9i4</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>My haul from the MoYou London sale on the stamping plates and polishes they're phasing out. An upgrade from the single plate I got from WalMart 💅</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dcw9i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ddy6oq</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My chemical romance nails I was inhaling the fumes for so long that I think a had a chemical romance with the nail polish </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddy6oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ddv5s1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at press ons and nail art! Made these for a friend and I’m praying they like them! Top row was the first go, a little easier the second! Took about three and a half hours! 🥰Used cat eye, black and white gel and some glitter for dots! </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jeys5gudq16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ddv56z</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Mom claims I “did the half moon wrong.”</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d8sx4s7q16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ddtv76</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>I don’t even wanna tell you guys how long this took 😅 BUT my cuticle work has improved a lot and I love how they turned out!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv6izxuee16d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ddt0vj</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>y2k meets bratz dolls?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddt0vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1dds6ql</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>First time working with white acrylic</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dds6ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ddq121</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Who Needs Juicy Strawberries?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5xihp0nui06d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ddpgve</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Newbie- using fake nails as canvas</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0qwygmme06d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ddpehq</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Any tips on how to get deals on professional brands or find quality dupes? For example: Sweetie Nail Supply</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ddpehq/any_tips_on_how_to_get_deals_on_professional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ddp534</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Advice FRENCH TIPS</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ddp534/advice_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ddot3l</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best ombre to date ☁️ </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddot3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ddl0ld</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Pride Set</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddl0ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ddjzpb</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">butterflies </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gm6pzlpaz5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ddgl39</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Update from Sundays post: here’s the final designs on my nails.</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ejmyqfdly5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1dddit2</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3D set by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/278c76okxx5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ddck7o</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Left handed rainbow nailart</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nezxwinox5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1ddcc9g</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Very new to nails/nail art (I first tried last month), this is my progress so far!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddcc9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ddc6gl</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>A fan-designed new hand-painted nail art! 🎨💅</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddc6gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ddbva0</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Me trying an ombré design and pearl powder</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wp2hfdwphx5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ddbowh</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>There aren't many nail patterns, plain colors : @aniisafar on ins Artist:https://www.instagram.com/aniisafar/</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ddbowh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun 13 08:09:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_16.xlsx
+++ b/data/2024_06_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C644"/>
+  <dimension ref="A1:C809"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11381,6 +11381,2812 @@
         </is>
       </c>
     </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1desy5j</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60lkil02ha6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1derwjd</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>One short nail</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9eawqkh4a6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1derq1e</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">meow  </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny6ng16c2a6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1derotv</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>black &amp; red strawberry nails 🍓🖤❤️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1derotv</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1derdc4</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Did my sisters nails, thoughts?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1derdc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1derb8n</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome powder recommendations for regular nail polish? 💅🏽 </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1derb8n/chrome_powder_recommendations_for_regular_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1der9kq</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>White Nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/13cpt5pnw96d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1der0d0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Opinions/ experiences with Ohora semi cured gel nails</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1der0d0/opinions_experiences_with_ohora_semi_cured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1deqyrb</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>My first time trying white. I went to Target and it felt like everybody was looking😭. Am I overthinking this or is white really that noticeable?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deqyrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1deqpyg</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Square French Tips</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deqpyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1deqivw</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Electric Forest ready ✨️</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjkjb35jo96d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1deph1z</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Which nails for my cruise??</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deph1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1depepl</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>I know these are simple, but I usually lean towards more simple designs… I’m obsessed with these right now and so happy with how they look.</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1depepl</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1dep1yo</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>gelx heat problem</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dep1yo/gelx_heat_problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1dep6h2</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed some stained glass cat eye nails rainbow for pride! </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dep6h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1deoz7e</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>UV Hard Gel Removal</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1deoz7e/uv_hard_gel_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1den3bf</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Nails weak!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1den3bf/nails_weak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1deofmx</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>My Berserk nails</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deofmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1deo6p6</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deo6p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1deo471</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Chrome blue nails 💙🐬</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deo471</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1denwvv</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>ISO Recommendations for Etsy shop</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1denwvv/iso_recommendations_for_etsy_shop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1dent5t</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Summer ✨</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42uexivvx86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1denki7</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Any suggestions for repair or strengthening a horizontal crack</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rx510ziov86d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1denh2a</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Haven't had my nails done in a few years 🥹 My girl brought me back beautifully ✨️</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q18ki2vsu86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1denejf</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>I don’t know what to do</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1re7yy4u86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1dena55</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>In search of gel polish brand in bottle with icon of sun circle and wave horizon, made in Japan. Macaron series as pictured.</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v26ts8fzs86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1den7da</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>3 days later… new set</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1den7da</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1den2ih</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY girls unite </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shhodojxq86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1den0cl</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail disaster </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1den0cl/nail_disaster/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1demz1o</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I have been trying to get better at doing my nails, I just finished these today :)</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1demz1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1demq3t</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I only have this photo of my natural nails from two years ago, and the french is my favorite, do you like it?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i757bremn86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1demjv1</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Summer Fruit Nails! 🍉🍋</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1demjv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1demkfu</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>how can i fix a terrible gel manicure at home?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3x5d8e5m86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1delwaf</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Un poco de color hoy!</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxf2m7e0g86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1delqit</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Decided to do almond/ oval shape on my nails for the first time by myself and I love them. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1delqit</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1del8qq</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Polish won’t stick to my thumbnail! Help!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tdd8r8aa86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1dekyra</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Salmonberries Nails!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dekyra</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1dekqyh</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I LOVE Kur’s Illuminating Nail Concealer “polish”</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr2l2bx6686d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1dekjcj</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Update: I ended up cutting it</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dekjcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1dekoh1</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>🐟🫒🍌🍓🫐🍉🍎</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7rlj46m586d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1deju4t</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Another Ladybug Look</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c1g8nity76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1dejpkl</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>I never get tired of basic nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dejpkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1dejfyn</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>My local grocery store had a huge box of clearance OPI and Morgan Taylor. What’s normally $7-$11 were all under $3!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0iganjiov76d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1dei7kn</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>How would you rate them? I’ve been doing nails for myself for about 2-3 years</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dei7kn</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1dej99x</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Nails turning different color</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99n4qra8u76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1dej8db</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Mooncat in The Most Destructive Melody</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/asvkcm91u76d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1dej3t1</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>A lil  winter pick n mix set</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dej3t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1deiwm7</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>🧡🩷💜💙💚</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deiwm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1deims4</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xymjmndp76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1deidxb</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deidxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1dei1wa</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>i love this set so much!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dei1wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1deh3oc</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Pink chrome polka dot🩷</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dhgp9tnd76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1degniv</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>My nail evolution</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1degniv</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1degaxe</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Big toe nail is going to be removed ideas to make my feet look nice?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1degaxe/big_toe_nail_is_going_to_be_removed_ideas_to_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1degpf0</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The pointier the better </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blvhz6doa76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1degidk</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1degidk</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1defqif</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defqif</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1defogf</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I have no idea how to heal my nails.</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defogf</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1defnhf</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Is it supposed to be this messy after?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defnhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1defks2</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Jobs that I can have long nails with</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1defks2/jobs_that_i_can_have_long_nails_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1defi8r</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my instructors nails today! </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defi8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1deff7m</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>I've been growing my nails and i want to start painting them, any tips?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deff7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1dee9l3</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Are my nail beds too flat for press ons?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dee9l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1def4fq</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Should I switch to personal nail tech?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1def4fq</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1def341</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Y2K Vibes</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1def341</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1deex6m</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where to buy good nail glue for rhinestones and little decorations?  </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1deex6m/where_to_buy_good_nail_glue_for_rhinestones_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1deeq69</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>(Advice) How to ask for translucent/jelly nails?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1deeq69/advice_how_to_ask_for_translucentjelly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1deeg39</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>My nail tech is so talented</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deeg39</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1deehc7</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>My kid asks me to “make their nails long” all the time. We now have cat claws</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deehc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1deecg8</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>My summer nails 🎀</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2sgm2g9t66d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1dedriu</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>ISO: A thick, gap filling nail glue</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dedriu/iso_a_thick_gap_filling_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1dedgjw</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>New claws</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2awms30tm66d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1dedcbg</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>my beautiful nails 💕💅</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redgifs.com/i/mildsecondhandaustraliancurlew.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1decync</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>I’m late to the party but I only just found out about chrome nails and now I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph517zt5j66d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1decvap</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Nail charms and glitter</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1decvap/nail_charms_and_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1decrex</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural gel nail manicure </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q6iek1oh66d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1de1ccp</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icegel </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt3j9beol36d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1de7wwx</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>How do I fix my broken?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnatm2dch56d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1deazrz</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Nail progress from March 2024 to now</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja9y0z8i466d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1de8qu0</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Often disappointed with bail length after appointments - unfair expectation or bad studio choices? </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1de8qu0/often_disappointed_with_bail_length_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1de8jq2</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>How do i grow back the pink parts of my nail?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1de8jq2/how_do_i_grow_back_the_pink_parts_of_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1de76r3</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Yellowing nails</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de76r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1de63l4</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Got these nails a week ago and still can’t get over them✨💅🏼💕</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1zrtzjp256d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1dearuq</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Practice makes perfect 🤞🏻🩵</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dearuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1deajan</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Which your choice for the summer mood?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deajan</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1deaerd</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>In love with this set I did🩵🌤️</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deaerd</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1de9z8r</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>How much should nails cost?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de9z8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1de9o7m</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Did these last night 🍊💅</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de9o7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1de9nfr</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>🌌</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi6merfiu56d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1de9fj1</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>💧💚 LOVEE THEM!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkd3ai1ss56d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1de8y4l</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Cat eye chrome ombré 💅💅💅</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9pju4xy5p56d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1de844o</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>I love this shade of red</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2gz113vi56d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1de7xm7</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Finally nailing my own nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de7xm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1de6meq</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Told my mom about this sub and she insisted I share her nails with y’all!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de6meq</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1de6kzc</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>What’s wrong w this nail design ?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de6kzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1de6fa1</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yes, I work. </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/88cuinc8556d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1de69bq</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Trying my hand at Press Ons!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de69bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1de5yvx</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Lemons or corn on the cob?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xqrfkdk156d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1de5y12</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last couple sets, self done GelX and Acrylic. </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de5y12</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1de5u8h</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>My own nails + hard gel</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmoc88se056d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1despuu</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Turquoise meets toppers</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ScBuixq</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1dequvo</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>My first time trying white. I went to target and it felt like everybody was looking 😭. Am I overthinking this or is white really that noticeable?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dequvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1deqehl</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Any tricks for making polish last longer?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deqehl</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1deq47h</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>BKL Sunbird</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deq47h</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1deq428</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>What am I missing?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deq428</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1dephy1</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>im ba-da-ba-ba-baaaaack</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dephy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1den9cl</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Jior Cotoure - Nom Nom Nom</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cscrct0rs86d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1den39q</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>BKL "Nevermore" + BKL "Nazayun"</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1den39q</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1demhnl</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>A palette cleanser with a little *pizazz*</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1demhnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1dembej</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Dupe request! Ethereal Lacquer "Star Children"</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dembej/dupe_request_ethereal_lacquer_star_children/</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1delw8h</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>🩷💜💙 Bi Pride Nails</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1delw8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1delgxr</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>🎟️🌞📀</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sm366l49c86d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1dek8yj</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Bluebell shorties</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dek8yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1dek038</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>It was reduced, so I had to buy it. Even though I already have similar colors.</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcc5uaq4086d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1deimey</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Think this is my new favorite color </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgw8nwuap76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1dehlfx</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Hot or cold?...One hand each heheh 💖</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dehlfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1dehkwa</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this the next plateau of exquisitely detailed nail art? </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/p/C8HZUHrscWu/?igsh=MWR2cWl5YWl1c3BxaQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1dehhg6</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green and purple felt like the hulk. Purple and orange felt like a collegiate sports team. All three together? Makes me happy. </t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv3rpr0jg76d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1deh6sd</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cost effective hema free systems? </t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1deh6sd/cost_effective_hema_free_systems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1degj79</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Lost a gel tip and now I feel…stubby</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0kmyf9ld976d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1degejo</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Recommendations for nail drill education?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1degejo/recommendations_for_nail_drill_education/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1deg9kc</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Annoying bent finger</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deg9kc</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1deg4a6</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Sharing given some neutral request posts...</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deg4a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1defs3f</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Growth check up, thank you to this page I can actually get my nails to grow ✅💚</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defs3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1defhu0</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>What is considered to be a successful, long-lasting manicure?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defhu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1deffrc</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Finally found my perfect neon pink 😍</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exye0gn9176d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1def0gm</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>✨House of Mirrors✨</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1def0gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1dedqkf</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Emergency patch on a nail break 🤕</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u70n3swuo66d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1ded7le</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Best polish storage option??</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ded7le/best_polish_storage_option/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1ded6m5</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Rainbow 🌈 Skittles Pride Set!! Do ya like the summer vibes? 🌞⛱️😎</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ded6m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1decyx6</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This mani is fabulous! Layering thermals is gonna be a new obsession </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1decyx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1decuyr</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Jelly/Crelly Suggestions?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1decuyr/jellycrelly_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1deasgh</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Ethereal - Darling Divine</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deasgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1deaiui</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Help finding color!!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1deaiui/help_finding_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1dea195</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>An older but a goodie!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gxwdyxex56d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1de9t8x</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Mooncat - When the Devil Strikes</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjam03hqv56d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1de9eph</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">van gogh almond blossoms! </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de9eph</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1de91hi</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Probably the most overdone polish of the year but I had to make a post 🤷🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de91hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1de6qp8</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Lagoon Jelly</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de6qp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1de684q</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>I think I like this pink 🩷</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de684q</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1de5umu</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Hypnotic is 😍</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdrwqvlh056d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1de5u4m</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>💜💛🏳️‍🌈Intersex Pride🏳️‍🌈💛💜</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de5u4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1de4h45</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Palate cleansers can be pretty special too 💘</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de4h45</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1de3yro</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Post-glitter carnage</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55eicg7zh46d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1de3r2y</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Cute drugstore Jelly</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de3r2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1de1pva</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Essie Lacquered Up Dupe</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1de1pva/essie_lacquered_up_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1derg0o</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Did my nails</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5fdptczy96d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1depjgc</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Best nail glue?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24qonelge96d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1deotxl</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Tried out a bunch of different designs as I brainstorm for a friend’s wedding nails</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52kfukbn796d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1denuhe</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Name of Design? Tutorial?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1denuhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1deicgl</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deicgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1dehv6o</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>New nail job</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46csp99ej76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1defozq</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Which one should I get for Summer nails?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defozq</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1defh49</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My instructors nails I did! </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1defh49</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1ded5vf</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Hello everyone! 🐰
+Do you enjoy creating characters with gel? I love exploring designs that require patience and precision. Each piece brings me so much satisfaction! Share your ideas for eye-catching summer nails with me. I'd love to hear them! 💅</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o6qo2bwtj66d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1deb0t6</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>First time w/ nail art and falsies. Trans theme for pride month</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuetzy8q466d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1deaq20</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>I did cats nails 😻</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deaq20</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1de9n2m</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Lil Yoshi egg 💅🏼💚</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de9n2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1de9dgj</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">van gogh almond blossoms </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de9dgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1de6njj</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Trying out press-ons!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de6njj</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1de5vas</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>My pride nails</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de5vas</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1de53by</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>First attempt at art</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdknwq9it46d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1de4ouc</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>did my nails!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de4ouc</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1de4mhh</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>My very first UV gel set!</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxq1wisyo46d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1de2u4t</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Lemon tree nail art!</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ig318r8546d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun 14 08:08:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_16.xlsx
+++ b/data/2024_06_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C809"/>
+  <dimension ref="A1:C983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14187,6 +14187,2964 @@
         </is>
       </c>
     </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1dflnqo</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Matte 💅🏻 spicing it up with a touch of colour ✨</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq6y98zjvh6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1dflmqx</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Thermo Colour</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8iii9l7vh6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1dflk48</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>New Gel Set 💖🍓💖</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dflk48</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1dfljh6</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Cover</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hl9wgr12uh6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1dflgbb</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Poisonous Nails </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dflgbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1dfkad4</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Gelnails lifting</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfkad4/gelnails_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1dfkucz</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Super cute</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz854kjykh6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1dfkq34</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Advice? I’m looking to improve</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvgmd28jjh6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1dfjlrx</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Happy about my progress!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfjlrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1dfk6p2</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try of airbrush </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfk6p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1dfjrhc</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>I love the way these turned out! What are your favorite nail wrap brands?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfjrhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1dfjjdk</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my derpy pokemon gel nails </t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfjjdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1dfj60y</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Guitarists: how do you wear your nails?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfj60y/guitarists_how_do_you_wear_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1dfh3zv</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>How do I take off these Gel-X nails?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfh3zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1dfha6r</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>🤡 inspired: nailssbycindyy</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7s9d50lwgg6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1dfje65</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Most difficult set I've ever had done. </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br403mvd3h6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1dfj9xk</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Bubble Gum</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfj9xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1dfj96b</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Which shape looks better on me?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfj96b</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1dfirko</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is in my MySpace top 8 for sure </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ls0v42k5wg6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1dfidug</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Can you use base gel or base coat as glue for Gel x nails?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfidug/can_you_use_base_gel_or_base_coat_as_glue_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1dfiayb</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Alternatives for the beetles nail glue?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfiayb/alternatives_for_the_beetles_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1dfhx1s</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>New work in progress</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxueedbgng6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1dfhpf4</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Hand painted Jujutsu Kaisen nails</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtdtfi39lg6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1dfhnic</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Hologram obsessed</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfhnic</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1dfhmvp</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Summer ombre</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfhmvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1dfhdum</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yay or nay! </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfhdum</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1dfh0kx</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Photo shoot set</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfh0kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1dfgurg</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Lil peep</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfgurg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1dfgm39</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>iso advice!!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfgm39/iso_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1dfgijw</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>my new nails🤍😋</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3un35bm99g6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1dfgi5w</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>my nails last month</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj5io2769g6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1dff6z3</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>how much would you have paid for these nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1ncyunrwf6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1dfgc5l</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Would rubber base be appropriate for me? What are recs for tutorials, items, brands, etc.</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfgc5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1dffp91</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Why do my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np5zukwm1g6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1dfggsq</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My nail tech told me today she is moving away… as I cry, please enjoy some of my favorite sets she’s done for me!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfggsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1dfgbxa</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question for nail techs </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfgbxa/question_for_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1dfg8zd</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>how much would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfg8zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1dfg72t</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Is it unreasonable not to want the top of my nails filed?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfg72t/is_it_unreasonable_not_to_want_the_top_of_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1dffyhz</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Where to get nail charms?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dffyhz/where_to_get_nail_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1dffj7j</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Peeling nails</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fi7b1bt00g6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1dffifh</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>This color is 😍</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sukarn8uzf6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1dff8kx</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Check out my wife's amazing nails, modeled after a lowrider chopper we saw at the Albuquerque super show. WorstSalonEver in Asheville. </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dff8kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1dff6yx</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Neon dip</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vouxnmrwf6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1dff316</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>🎀💝</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dff316</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1dfeuki</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>BF chooses my nail color - Part 2</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfeuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1dfcnte</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Is There A Non-Gel No Wipe Top Coat?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfcnte/is_there_a_nongel_no_wipe_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1dfcqwl</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>I am allergic to the UV light thingy but I really enjoy getting long nails.</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfcqwl/i_am_allergic_to_the_uv_light_thingy_but_i_really/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1dfejo1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Any cool semi easy designs I could do for pride? I’m marching in the parade and figured I’d go all out this year lol</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfejo1/any_cool_semi_easy_designs_i_could_do_for_pride/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1dfeb9e</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Dazzle Dry chipping super fast</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfeb9e/dazzle_dry_chipping_super_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1dfdshl</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>I want to develop healthier nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pokeuq4mjf6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1dfd8sy</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Some chrome French tips</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9tnphxjef6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1dfd6ep</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>I've been experimenting with my nails lately. My cuticles are begging for mercy, how can I protect them?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq34rs39ef6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1dfd648</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>New set 🤗</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfd648</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1dfd5oi</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink and flowers </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvwmbjp2ef6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1dfd0nn</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Acrylic/ dip/ sets always look too thick to me</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfd0nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1dfcxr3</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Best pricing for press-ons?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfcxr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1dfco8x</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Nail progress!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfco8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1dfcnwm</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Pink/nude nails</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfcnwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1dfcnv3</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Help after gel!</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5l8foh9u9f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1dfcd8m</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Pretty in pink 💅🏽</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4t2jnlnc7f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1dfccpe</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails and tips </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfccpe/press_on_nails_and_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1df9s7w</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Why does the builder gel always peel off my nails</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dih7ibseme6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1dfc65k</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Is doing your own nails count as a hobby?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfc65k</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1dfc0cv</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Simple but sgood. My girl always kills it ✨</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o5ad88g4f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1dfbzk1</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Siren Nails</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltbzu5l94f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1dfbspa</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>I like this soft pink, do you like how they look?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfbspa</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1dfbski</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>June nails!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tamnkkgm2f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1dfbsb0</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Nails of the month :)</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfbsb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1dfbq55</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Encapsulated flowers 💐 </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yamf9p22f6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1dfbmzf</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>I’m a complete beginner to gel nails - my first manicure using tips</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7me1bgmc1f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1dfbin9</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>It’s been a while!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0y105yc0f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1dfbfbp</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>are these cute to get for pride month or am i tripping?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brd0p1tkze6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1dfb6ap</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>I was given this and couldn’t find instructions anywhere , do I need to cure it?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nl2zspgxe6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1df9td8</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Happy Pride, y’all!</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df9td8</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1dfab5q</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Sets I’ve had done 💅🏼💅🏼</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfab5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1dfa9jv</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>New mani!</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu1figf6qe6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1dfa3n6</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>First Set of Pride Nails of the Season</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfa3n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1dfa0s4</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>'22-'23 nail growth journey from start to finish ✨</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hyjxk9n9oe6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1df9vnx</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Breaking nails</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5w6jug5ne6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1df9suj</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Nude color recommendations?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df9suj</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1df94m1</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting acrylics, nervous </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1df94m1/first_time_getting_acrylics_nervous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1df9kv7</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Is builder gel easier than biogel as a beginner?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1df9kv7/is_builder_gel_easier_than_biogel_as_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1df9id1</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lil Glazed Donut Moment </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zk6qlrbke6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1df9gix</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>First time doing a manicure ever. Gel nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rdex3lxje6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1df9els</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>First time getting Gel-x extensions</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auzfx2pije6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1df8j65</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>My first time getting my nails done in 10 years.</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0iozmvxce6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1df8ivq</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>💚 Cirque Colors All In 🧡</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df8ivq</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1df8iiw</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>I think I've got my cuticles under control but I'm still struggling with shaping</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df8iiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1df87ta</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>How much do you usually spend on your nails?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idc7sjslae6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1df883f</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Pinterest made me do it 😂</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7sp40rnae6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1df8b08</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My first set for myself this month 🥹</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajzebu18be6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1df8ah1</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Cherry, cherry lady🍒</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df8ah1</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1df87am</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>First time getting creative...</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df87am</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1df7vep</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Someone needs my attention </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mbng8vty7e6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1df7qx5</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like my cuticles are always all over the place </t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1df7qx5/i_feel_like_my_cuticles_are_always_all_over_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1df7lyr</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Pride UFO nails 🌈 🛸</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df7lyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1df7lf6</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Tropical frog nails</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df7lf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1df7k3e</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Tried green nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysm0823j5e6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1df2kus</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Dropped a weight on my nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex8yaxj54d6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1deqiw0</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Nail inspo?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deqiw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1dfk9xa</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Does anyone know a dupe for Cafe au lait by Sally Hansen?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clq9fhvudh6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1dfk8ri</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hope we’re still doing the goofy pose thing cause I can’t get enough </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfk8ri</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1dfinis</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>super dumb question about gel</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfinis/super_dumb_question_about_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1dfhor6</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Polishes similar to flower child?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfhor6/polishes_similar_to_flower_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1dfg1c1</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Nebula Garden ✨</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m8w857dp4g6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1dfftwq</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Possibly overfiled my nails but still want to use press ons</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfftwq/possibly_overfiled_my_nails_but_still_want_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1dfemeh</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Unfortunately my nails are too short to show off the multi chrome, but I still love it irl (Prince of Hearts, BKL)</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfemeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1dfehv0</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Flower Child 🌸</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfehv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1dfdtd2</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Anyone else desperately trying to get every possible crème shade to make better skittles?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfdtd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1dfcoak</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>I ruined this mani about ten minutes after these photos were taken</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfcoak</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1dfchou</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>One of the best summertime blues 💙 Serenity</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfchou</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1dfc584</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>I wish this mani could last forever</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/NwvMuZc</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1dfc187</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>🌙🌈✨💅🏻☁️♉︎</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zno6r6m4f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1dfbrep</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Tried green nails for the first time and am loving it!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l51x74hd2f6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1dfbhuj</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Best NON quick dry top coat with no shrinkage?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfbhuj/best_non_quick_dry_top_coat_with_no_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1dfb9f6</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Subtle but cute ✨</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfb9f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1dfa1sb</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Mooncat To All Who Ghosted Me</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/007vg09ioe6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1dfa0ef</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Help me recreate this look with Laquer</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8cabm47oe6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1df9j23</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lil Glazed Donut Moment </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j663ua8hke6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1df9hhy</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Queen of Rot</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df9hhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1df8uwt</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jior Celestial Goddess </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df8uwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1df8llc</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is your preferred method of swatching your polish collection? </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1df8llc/what_is_your_preferred_method_of_swatching_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1df8i4h</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>💚 Cirque Colors All In 🧡</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df8i4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1df88at</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I want gel nails but I dont know if it’s realistic</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df88at</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1df71q6</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Happy Pride 🌈</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df71q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1df6ed0</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Feeling peachy 🍑✨🧡</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycswvh6xwd6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1df64z1</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice needed! How do I make this stop peeling so easily? And how do I make this not so thick? I keep flooding my channels and this peels in two days after I do it. </t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df64z1</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1df5sc1</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Removing regular polish from Gel X nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1df5sc1/removing_regular_polish_from_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1df56eb</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Ethereal - Moonbeam</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df56eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1df531w</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Summer ferns and flowers</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df531w</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1df4y16</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>ILNP Summer! And My First KB Shimmer</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fez2ud2md6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1df4p5u</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>HoH post no.9472…</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcsr5qf6kd6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1df4hyo</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Kb Shimmer / hidden potential</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df4hyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1df4cwl</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Pain from OPI Repair Mode</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1df4cwl/pain_from_opi_repair_mode/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1df3rlb</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Royal Blue Gel</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9pjv5c3dd6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1df3ki3</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>I’m so jealous of your press ons 😭</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6gt90hlbd6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1df25xr</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Lesbian Flag: Pride Flags for Pride</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df25xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1df1vad</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>2 pix, help me pic</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df1vad</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1df1nfd</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Move over Holotaco there’s a new holo queen in town</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df1nfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1df11q0</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Polish search</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1df11q0/polish_search/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1deztrf</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Light blue magnetic </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1deztrf/light_blue_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1deznrj</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Hitting angles feeling like a professional swatcher</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deznrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1deyf4h</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>It's like having my own laser show</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deyf4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1dey6i5</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Sublime.</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ynyz6xd5c6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1dexf80</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>🖤🩶🏳️‍🌈Aromantic Pride🏳️‍🌈🤍💚</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dexf80</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1dex0al</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Any experience with polished for days?</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s77hyhq0ub6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1dew8i7</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a good prugly </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dew8i7</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1devsrw</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Bought this for 60 pence and it's almost a great dupe for Bikini So Teeny - get on it thrifty UK polish fans!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdutkv6ugb6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1deup08</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Glitter skittle nails (sorry for the shaky video, I was having a hard time with it but really wanted to show the sparkle) - they are an absolutely pain to remove on my natural nails, so this time I wanted to do them as press-ons</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deup08</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1dekcnv</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>les gusta?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/aBkLzMv.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1deifdj</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>ILNP- Eclipse</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/149engbrn76d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1de83d2</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Fun with thermals 💅🏻</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1de83d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1de581n</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love at first sight </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6jnjmiqu46d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1dfjz2g</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Pride 2024 Nails - Natural nails, art by @kalsrebelliousnails on IG</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/PM5HTNj</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1dfjv92</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>I did these in class so far</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfjv92</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1dfi3js</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>I worked 3 hours but they turned out beautiful</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qci0d18pg6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1dfgju1</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long lipstick press-ons </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o3yn8nyl9g6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1dff05l</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>The nails i made this month</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dff05l</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1dfdwhm</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>3D nail art</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfdwhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1dfdgmm</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Today ✨💜</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfdgmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1dfau54</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pastel Goth set - ombré with stamping details </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfau54</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1dfai61</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>I love a bit of Pinterest inspo!</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfai61</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1df9s6o</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Little duck 🌸</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v86abzgeme6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1df9ir5</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Painted my nails fun today 🦑</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vs371veke6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1df7a5z</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Sparkly floral pedi</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1df7a5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1df5hlw</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qfnqa55qd6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1df540o</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>How to create 3D nail art with nail polish? (not gel⚠️)</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1df540o/how_to_create_3d_nail_art_with_nail_polish_not_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1df48fn</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Sleep token nails</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkhqo9ilgd6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1df4673</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>if you'd want some inspo y'all</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3wr0h8wfd6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1df42eh</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>One Stroke</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1df42eh/one_stroke/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1df2p1d</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Nails of the day</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dj5w2m15d6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1df1fxo</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did kuromi nails! </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jbbzg3pivc6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1dewk3z</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Dotty Cherries</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dewk3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1deukts</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>LEGO nails because.... wait do I need a reason for LEGO nails? Insta - @charli.bell.9</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1deukts</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun 15 08:08:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_16.xlsx
+++ b/data/2024_06_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C983"/>
+  <dimension ref="A1:C1159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17145,6 +17145,2998 @@
         </is>
       </c>
     </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1dgcjkp</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>My wedding nails 🕊</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2adukg0uo6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1dgbqul</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Swirly grey</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23d80e97ko6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1dgbi8f</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Gel overlay</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgbi8f/gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1dgavxp</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A few of my sets </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgavxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1dga9z9</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>New set!! Inspo from https://pin.it/1O1E3WCjg</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dga9z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1dgb7hl</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Still learning, but this is the best nail art art I've been able to do so far!</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p54hn4ypdo6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1dgad41</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>My chrome is not shiny enough</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncez5wtr3o6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1dg9x7a</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SoCal nail tech </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3btbt1uyn6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1dg9dto</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>How to keep base coat and top coat on for longer than two days?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dg9dto/how_to_keep_base_coat_and_top_coat_on_for_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1dg9qlx</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Alcohol ink set</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02vd9h2swn6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1dg9qjj</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Just because nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1t9chntwn6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1dg9l44</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love orange! </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmk8a4z6vn6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1dg8zyg</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Zebra</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg8zyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1dg8xz0</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>I love my press on nails</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg8xz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1dg8xfu</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Clear coats with gel polish</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dg8xfu/clear_coats_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1dg8pzw</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Feeling fruity 🍓🍍</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg8pzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1dg8k9h</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling very summer right now with my frutas mani and pool floats </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg8k9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1dg8cax</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Got my full set for the summer 🧡🩷💛</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nigupdt6in6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1dg8bqq</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>My Nails and My Mental State</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dg8bqq/my_nails_and_my_mental_state/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1dg75dl</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Help darkened lateral nail folds</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcxlerwc6n6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1dg6ph5</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>The Nails Bae Pink Chrome Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5j2skmfz1n6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1dg7y1c</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Feeling Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg7y1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1dg7keg</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Magnetic nail polish that looks clear/transparent?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg7keg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1dg7iug</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>I love a good nail day 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg7iug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1dg75rz</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is an old set, but it's one of my favorites. </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg75rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1dg68us</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Set </t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61c925sixm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1dg5t1p</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>What's Your Go-To Neutral Nail Color? Let's Share Our Favorites!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dg5t1p/whats_your_goto_neutral_nail_color_lets_share_our/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1dg5rlt</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1oibgt31tm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1dg5hsi</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>How to fix a (gel) broken nail</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg5hsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1dg545q</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Does this work?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2vw0642nm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1dg4rd0</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>My nails for pride month!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg4rd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1dg4ke2</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Red always makes me ready for summer ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7642r04im6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1dg4i4r</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>My pink nails i love it 🥰💋</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k8ymctjhm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1dg4bjn</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Any tips on keeping nails from breaking off?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg4bjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1dg4366</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>showing off my pride and joy, my natural length!!</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ppfe4rwdm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1dg3afj</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PNF is not the cuticle </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t3sr6997m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1dg3wxj</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Went a tiny bit longer this time!</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx4vvececm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1dg3vt6</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>My nail tech did amazing on this set</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv232dt4cm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1dg2at6</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Advice for Nail Injury</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg2at6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1dg3k1d</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>I like them</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs24rnei9m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1dg3iv2</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Nails for a work event!</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg3iv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1dg3h2z</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Black, the basic</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wiba3pus8m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1dg3fmu</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Who else loves contrasting nails? :3</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zikxbz88m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1dg3ew2</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Girlie Summer Set</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ausdxrna8m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1dg2v57</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Some people call me the space cowboy</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg2v57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1dg2plz</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Help with press on nails</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhn95edf2m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1dg2ecn</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>My naturals nails , just acrylic on them 😍🥰</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z82rh9gtzl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1dg2de1</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Was eating strawberries, got obsessed 😂🍓</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg2de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1dg28ul</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>what do you think of my nails?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6571n1ziyl6d1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1dg2794</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>First time diy acrylics</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef66m8m6yl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1dg1nw8</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Fixing damage after first time builder gel polish?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dg1nw8/fixing_damage_after_first_time_builder_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1dg1uxi</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do your natural nails survive when regularly getting nails done? </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dg1uxi/how_do_your_natural_nails_survive_when_regularly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1dg067y</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Need your help ! Wtf is this ?!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xdqdm83il6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1dg1kh6</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some Nail Inspo for your feed </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg1kh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1dg1k2c</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>super cute nails i got about a week ago 🫶</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2x6spwzsl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1dg1kxq</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Mooncat Ultrahot</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg1kxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1dg1iwc</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Not exactly what I had in mind but still cute!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg1iwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1dg1a92</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>My ally set</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg1a92</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1dg13zj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Love a simple almond set🤍</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nuvkb58ipl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1dg102b</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Is this not the most beautiful color you've ever seen!?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5rwotzlol6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1dg0p9i</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>they like?😟</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io1s5od8ml6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1dg0n7q</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>New nail tech killed it!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg0n7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1dg0id8</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>My 3rd time doing gel x!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqyn08ynkl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1dg0b1x</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Went for a short lunch run and could not stop staring at my nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vbrrr6y3jl6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1dfz5wp</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Chappell Roan inspired nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt463q68al6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1dfzkx7</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Can anyone help me find what this discontinued nail polish was? Or its story/color?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfzkx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1dfz9b0</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>What do you think of my natural nails?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tra5y5pzal6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1dfz66l</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Need nails that will look decent for a 3 week holiday - acrylic or gel?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfz66l/need_nails_that_will_look_decent_for_a_3_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1dfz1a9</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>does this shape/colour suit me?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kt5lbd79l6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1dfyx12</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>birthday nails</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfyx12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1dfyogf</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>bubblegum sparklessss</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfyogf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1dfylty</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for this color </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfylty</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1dfygj0</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Very different than my usual sets. I was feeling earthy I guess lol I think they came out cute 🤗</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfygj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1dfya6m</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Super proud of this set! Finally figured out builder gel.</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfya6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1dfy9hp</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Purple Power 💜</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyqz4c113l6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1dfxhdz</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wrecked my nails </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfxhdz/wrecked_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1dfy1bq</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>I always get a French manicure for my birthday</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi95zc091l6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1dfxzy5</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Summer Pedicure</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7291e26x0l6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1dfuw1z</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfuw1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1dfvl50</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Better warm or cold??</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfvl50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1dfxkf9</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Advice on what type of set to choose</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfxkf9/advice_on_what_type_of_set_to_choose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1dfxwff</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>help me create a nail set for my mom please</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfxwff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1dfxouz</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Nail wraps and Gel X?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfxouz/nail_wraps_and_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1dfxjce</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Daisy nails!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfxjce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1dfxi4w</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eras tour ready! (nails by me __kmnails) </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqlilpv5xk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1dfx4px</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Second time I got my nails done 🖤</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtix6o7auk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1dfwc1o</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Pedicure questions</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfwc1o/pedicure_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1dfws33</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I grabbed the wrong nail while using press ons… How do I get it off so I can use it on the right nail? Or am I just screwed 😭</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0962buylrk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1dfwaqa</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Icy, watery, and shiny nails!</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5sr1tuwunk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1dfw2hi</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Red!</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qz11q33mk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1dfvws9</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my nails again for the first time in ages! </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/higsv1ovkk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1dfvj2k</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfvj2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1dfvixc</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>how to ask nail lady for this</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dfvixc/how_to_ask_nail_lady_for_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1dfvetg</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>I was not ready</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ds1gvg7zgk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1dfv39q</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tubq5igiek6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1dfus88</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>I’m in love with these!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t33sfg74ck6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1dfurpd</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>I've been growing my nails and i want to start painting them soon. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfurpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1dfqogn</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Thanks to my last post and all you wonderful people, OPI reached out to me and sent me these beautiful nails. Thank you, all of you, for helping me help others.</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfqogn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1dft42n</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>I broke a nail. Tips for a road to recovery?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dft42n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1dftmsd</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>How to prevent lifting?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dftmsd/how_to_prevent_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1dgbdds</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>It is the color that is fashionable in my city! It is from the nude line from the Cleopatra brand 💖</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgbdds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1dgappi</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>How do you keep your natural nails long, strong and peel /chip free</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgappi/how_do_you_keep_your_natural_nails_long_strong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1dg9o9x</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Anyone ever take polish thinner on a plane?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dg9o9x/anyone_ever_take_polish_thinner_on_a_plane/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1dg5bfc</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">chanel rose confidentiel dupe? </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q07mc5ttom6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1dfyzux</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>BKL question</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfyzux/bkl_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1dfvnke</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Impulse buy at the airport made for a nice cream HoH dupe</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfqokm1xik6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1dg8ufp</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Finally went almond-shaped</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg8ufp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1dg8niy</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manis at work today! </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg8niy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1dg7yp9</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Summer Fruity Nails</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg7yp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1dg7qfq</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guided by the Light ~ Vanessa Molina ~May PPU </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg7qfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1dg78v3</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Is there a way to tell if a polish/lacquer is sheer without opening it?</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dg78v3/is_there_a_way_to_tell_if_a_polishlacquer_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1dg71q8</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Brought my frutas mani poolside</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg71q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1dg6uoq</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>It's not the best, but I did my nails like Is from Kamen Rider Zero One</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fe8kt3f3n6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1dg5dni</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Longwear dupe for OPI Virgoals?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg5dni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1dg54fs</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What drops did everyone participate in? </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dg54fs/what_drops_did_everyone_participate_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1dg4ee2</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Severe nail bed damage &amp; pain - please help!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2gmftqmgm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1dg4bw7</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>I'm obsessed with this sparkly pink color</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg4bw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1dg44a4</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blåhaj nails 🦈🩷🤍🩵 </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg44a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1dg3vqv</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>SWAMP GLOSS / BCB LACQUER UPDATE</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dg3vqv/swamp_gloss_bcb_lacquer_update/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1dg2sf2</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Not HoH</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg2sf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1dg2qs6</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Red-Holiday-Beach-Vibes</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtk3k61p2m6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1dg2iuf</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Kur Perfecting Nail Veil #3 - Mauve??? Nope!</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dg2iuf/kur_perfecting_nail_veil_3_mauve_nope/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1dg2gvy</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Does anyone know of any multichrome top coats with clear bases like Shimmy Shake (sold out) by Sassy Sauce Polish? Not sure what to search for/what to call a top coat like this. Doesn’t have to be this color</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg2gvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1dg22cp</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unicorn Pride </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcgvcmn3xl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1dg22b6</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Berry porridge inspired 🍓🫐</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg22b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1dg1lxq</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Speckled pebbles on my fingertips </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg1lxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1dg02kp</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Funky combo!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg02kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1dfzlpt</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Brucie 🦇✨️</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfzlpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1dfz3wn</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL question </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfz3wn/bkl_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1dfyk6o</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>ILNP Mega L</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfyk6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1dfyfv2</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Shaka 🩷 Pink/red shimmer </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfyfv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1dfxr2d</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Amazing Pink</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/XzABxJw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1dfxd0v</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ERAS tour ready!!!! nails by me (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrt2p4h2wk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1dfxaj1</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Minimalist nail art </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5gki2ajvk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1dfx331</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Avoid Nails Inc glitter toppers</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cn8ayn8ytk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1dfwvr2</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>what are the best brands?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfwvr2/what_are_the_best_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1dfwrzo</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>LYN B. Designs 50% Off With Code BDAY Until June 21st.</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfwrzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1dfwjhr</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thxu68trpk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1dfwhk0</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Pure Ice ✨💖🪩</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfwhk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1dfwcq1</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nail art brushes</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfwcq1/nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1dfvx8o</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>💙💛🏳️‍🌈Pan Pride🏳️‍🌈💛🩷</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfvx8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1dfvpxf</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Red Black Polish</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uchvkp1ejk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1dfvmdb</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>A bit late for a pride mani but that’s ok cause rainbows are cool any day of the year 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaj1qs5nik6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1dfvizw</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>I can see why this polish gets no love…</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfvizw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1dfuwqp</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update w/ video - OK, y'all were right... </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5x0k7mj2dk6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1dfuc6z</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>All I did was open a cabinet 😭😭</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohc079po8k6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1dfu2l9</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>My first Death Valley purchase!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfu2l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1dftwtw</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gold flecks Stratosphere </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dftwtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1dftrx6</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Using an Allen wrench to put a bookshelf together while wearing Cirque Color’s Terra and you can see pretty clearly which of my fingers were exerting the most force! I usually have poor circulation so my thermals tend to stay at the “cold” setting. </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byrxjeo14k6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1dfthvi</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>BKL must haves?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfthvi/bkl_must_haves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1dfthgo</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Emily de Molly polishes? </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfthgo/best_emily_de_molly_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1dfsxkd</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta Dri- Peachy Breeze</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bho2t88zxj6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1dfslpw</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Decided to take everyone’s very wise advice and stick to polish for the foreseeable future! Thanks you guys are the best!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfslpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1dfslnp</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>I was not ready</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s414vlfvj6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1dfsiuv</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>💚🩷</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfsiuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1dfqsx1</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Disappointed 🥺</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfqsx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1dfq1db</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is OPI glass nail file made with czech glass? </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dfq1db/is_opi_glass_nail_file_made_with_czech_glass/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1dfpwft</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>💜💚 Spring Flower Vibes</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfpwft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1dfp5hm</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>I tried something new</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfp5hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1dfn741</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>When you make a product for the nail community and an influencer loves it! (Review link in description)</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/old67nrofi6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1dfm5kl</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Darling divine 😍</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfm5kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1dgaqkm</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Second pride set !🌈🥳</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgaqkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1dga2n9</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>An alcohol ink set</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ajv6reh0o6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1dg663c</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Just a few designs I did today.</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1p6v66gtwm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1dg43w3</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Super proud of this set. Did it in 2 hours!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8km1y203em6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1dg3sz1</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Nails of the day 🥵</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjli2uugbm6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1dg3ano</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>I dunno about these, what do they need?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dg3ano</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1dg2abc</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Hand painted 90s themed set!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gahzg71wyl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1dfzte3</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>A little calf</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcbly3zdfl6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1dfylut</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Muah 💋</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfylut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1dfyhj3</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Very different than my usual sets. I was feeling earthy I guess lol I think they came out cute 🤗</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dfyhj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1dfyavy</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Purple Power 💜</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8oxa66c3l6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1dfxirz</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Eras tour ready! (nails by me __kmnails)</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i5fiudaxk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1dfvq7v</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>What do you think of these?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd3mf5tejk6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1dfsqsr</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Does anyone have any idea on how I could execute this for nail art?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0qj767kwj6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1dfp5ww</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>they like this design?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu5ib33w1j6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun 16 08:07:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_16.xlsx
+++ b/data/2024_06_16.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1159"/>
+  <dimension ref="A1:C1325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20137,6 +20137,2828 @@
         </is>
       </c>
     </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1dh2sf2</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>My new nails. It costs 10 US dollar in my country :)</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dh2sf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1dh2q4p</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>New to Gel</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azoc857f4w6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1dh2pic</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Was going for elegant!</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dh2pic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1dh1pwp</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Help! Manicurist left me with raw &amp; red cuticle</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/648w23narv6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1dh2d83</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Feelin’ blue</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kidii2mzv6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1dh1cnn</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>how to repaint over my acrylics?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dh1cnn/how_to_repaint_over_my_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1dh14qj</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Music festival nails 🫶</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dh14qj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1dh0icx</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Need advice on polish vs gel</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dh0icx/need_advice_on_polish_vs_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1dh0vkn</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Really loving this set I did 🩷</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnphomglgv6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1dgr8hx</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with cuticles! </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgr8hx/help_with_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1dh0lgl</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>French tips ✨</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecdklxy9dv6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1dgytd1</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>What do we do about the dead skin accumulates on both sides of the nail toward the end of the finger?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6oywtj79tu6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1dgymbj</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>second attempt at mermaid nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgymbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1dgyjep</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>🩷💛💙 Nails</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgyjep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1dgyewx</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>my natural nails 3 months after cutting them (:</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgyewx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1dgso2r</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Has anyone tried these?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgtubc7x4t6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1dgtglu</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Damage after acrylics</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgtglu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1dgxr3g</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Stone/water nails</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgxr3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1dgyb1q</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Color changing purple flower nails</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgyb1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1dgxxit</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Strawberry nails 🍓</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgxxit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1dgxtpj</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Dupe for Sorry, Not Sorry from Lights Lacquer?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgxtpj/dupe_for_sorry_not_sorry_from_lights_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1dgxrej</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>First time ever designing press ons!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1zcw7azhu6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1dgxktv</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pride nails 🌈 </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgxktv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1dgx7ha</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Update on my husband’s Japanese manicure (2 weeks of growth)</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgx7ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1dgx78a</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summertime ocean theme </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgx78a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1dgtwy9</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Out here looking like a snack</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgtwy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1dgw7fy</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Switched it up a bit 💅🏼🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9nxkv522u6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1dgw479</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>More flowers and gold</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/seh73qf71u6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1dgw13y</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Forever a square frenchie nail girl 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upk4v1lb0u6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1dgvtxk</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Periwinkle powda!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zr3s1cxbyt6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1dgvskt</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>First time trying dip on my natural nails ✨</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ujo8mfyxt6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1dgvs9f</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Which hand looks more like "pool water"</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgvs9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1dgvjl0</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Is the mod team okay with this subreddit used to advertise foot fetish accounts, thereby making the subreddit unsafe for regular users because it attracts foot fetishists?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgvjl0/is_the_mod_team_okay_with_this_subreddit_used_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1dgvgpf</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvg56beout6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1dgv7kl</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Fresh nails 💜</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rujh6c7st6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1dguxqc</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Recent sets done!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dguxqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1dguljz</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>gelx tips for curved nails?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dguljz/gelx_tips_for_curved_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1dgucxb</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Summer Fruit Nails 🍉🍋</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgucxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1dgu41a</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Is this normal for short acrylics??</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgu41a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1dgu1o7</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>can i ask the nail tech to not fully fill one of my nail beds to the edges?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgu1o7/can_i_ask_the_nail_tech_to_not_fully_fill_one_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1dgt86t</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Flower Garden</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgt86t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1dgszn6</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>fresh set 💅🏽🤍</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zg53n88s7t6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1dgsy1s</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What color it is? </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldj24rrd7t6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1dgss6b</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>New set for Pride! Bi and Nonbinary flags</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgss6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1dgsqo2</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Watermelon Sugar 🍉🍉🍉</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/5UH07K7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1dgso94</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>When you’re obsessed with oiling your nails/cuticles…</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgso94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1dgsk8n</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Best brand of biab?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgsk8n/best_brand_of_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1dgsjqv</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⭐️ Mooncat polish in the color Pandemonium ⭐️ </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m0x8kryt3t6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1dgrxcw</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Always feeling green. 💚</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2hubifgys6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1dgr0ro</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Builder gel for UK (non nail technician)? </t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgr0ro/best_builder_gel_for_uk_non_nail_technician/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1dgqzi9</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>I’m afraid I slayed</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgqzi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1dgqqh1</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>how do they do it keep your nails so beautiful and maintain the color well? It never lasts and they break very quickly…</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgqqh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1dgqat6</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>New Salon, New Tech, New Nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phr0if7lks6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1dgqpdu</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Mermaid nails !</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgqpdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1dgqnb5</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Is there a difference between the two?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpjjltokns6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1dgqj0u</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>If i do my blue collar man’s nails, should i not cut cuticles?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgqj0u/if_i_do_my_blue_collar_mans_nails_should_i_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1dgqi6e</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Complimentary summer colors for fingers and toes? </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgqi6e/complimentary_summer_colors_for_fingers_and_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1dgq433</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After one week 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tk8enh2js6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1dgozmk</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Been going to the same guy…like his work but also not sure</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgozmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1dgos2f</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Happy summer nails</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlo1hugq7s6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1dgo9ry</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>What advice would you give for first time pedicure?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgo9ry/what_advice_would_you_give_for_first_time_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1dgo3qk</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>My first submission</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgo3qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1dgnig1</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>would you use this for gel tips or rubber base?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6obfh8l8xr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1dgn81a</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Why are nails are prettier when someone else pays for them?😀</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baqo6qosur6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1dgm1kb</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Gothic lick, more variants on the way</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m3382itkr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1dgki03</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>New set! 💜</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgki03</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1dgjlxp</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Nail thinning</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgjlxp/nail_thinning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1dgjepm</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Why does this always happen when I get a manicure</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl85yn4tyq6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1dgok9t</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Simple mani</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gywpot7w5s6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1dghmf2</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>What should I call this set? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5wgle8tiq6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1dgoard</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>What nails would look good with this dress? I’m going to a wedding in August wearing this dress. I’m leaning towards almond shaped nails 😁</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1z6zz1p3s6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1dgo88c</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Then &amp;, Now: DIY Nails</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgo88c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1dgo7n8</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>These are fun for the summer!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vzdnm4z2s6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1dgo1a2</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Change of Color and got a Mani. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgo1a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1dgnxnf</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Gelnails with Cateye</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgnxnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1dgnumy</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>So fresh… I love them! How’s the quality?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgnumy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1dgne0v</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>How could it be so beautiful!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iutmnxi6wr6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1dgncig</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>❤️Queen of Hearts❤️</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgncig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1dgn474</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>First Timer</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgn474</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1dgn2p9</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Blue Crush for Summer 🩵🩵🩵</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgn2p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1dgn28n</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>subtle pride nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inqbypwftr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1dgmts9</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Criss-cross bow set</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/750u6ywgrr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1dgmr4s</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Natural nails and their shape/ color</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xt3i5ejtqr6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1dgmr2l</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Gemstone set I did on my mom!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ih2b0vsqr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1dgmoq2</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>What color for my nail shape?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgmoq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1dgmfej</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Fun Summery Sapphic Nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgmfej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1dgmein</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>new set what do you guys think ? 💚</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgmein</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1dgm2lf</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/laq3m1f4lr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1dglz9n</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Simple minty set</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82w7dtvbkr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1dglk6i</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Complimentary colors - favorite combos?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dglk6i/complimentary_colors_favorite_combos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1dgl4x6</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>My favourite 90s cow print</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6fvor37dr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1dgl1n7</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>🥚Eggshell nails🥚</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgl1n7/eggshell_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1dgkt19</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Top coat for chunky glitter</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgkt19/top_coat_for_chunky_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1dgkppb</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Best nail shape for small hands and short nail beds?</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jz44uyl9r6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1dgko8m</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I usually have long almond shaped nails but I decided to switch it up. My nail artist killed it on the design! </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgko8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1dgkaig</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>The Gleeful Widow</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgkaig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1dgk699</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 weeks </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04uqyef45r6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1dgjrou</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Does anyone else scroll upward on their phone only to have it swipe left instead?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dgjrou/does_anyone_else_scroll_upward_on_their_phone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1dgje0f</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amber nails I designed </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwledywmyq6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1dgirpq</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>MOONCAT - Am I Everything You Fear?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgirpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1dgjjwi</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>I have been influenced!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9occpjy00r6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1dgz6em</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Jior Couture - Celestial Goddess (May 2024 PPU)</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgz6em</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1dgyrva</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Just had a bit of an epiphany about why lacquer means so much to me</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgyrva/just_had_a_bit_of_an_epiphany_about_why_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1dgxtyf</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>The bottle of Nightcrawler I ordered broke in transit so Mooncat was kind enough to send me another bottle… that also broke in transit</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ye7exfqiu6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1dgxshy</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>DVN’s West Texas Peyote w a little help from Vanessa Molinas Pitstop!</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgxshy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1dgxmeb</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Saturn 🪐enamelled with milky way and little French black cleopatra brand 💞</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcwjh9chgu6d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1dgxfhd</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Jelly sandwich ideas?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgxfhd/jelly_sandwich_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1dgxe2l</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about Cuticula’s monthly subscription </t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgxe2l/question_about_cuticulas_monthly_subscription/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1dgvi63</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lil pride nail 🏳️‍🌈 first time trying art 🫣 </t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xume3w2vt6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1dguvm7</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Swatching you . . . Swatching me</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dguvm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1dgulv6</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>New gel-x set, I ended up hating the orange/brown color.. can I paint over it to change the color?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq6o1figmt6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1dguj9z</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Summer Fruit Nails 🍉🍋</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dguj9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1dgtlg4</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Mid-Mani Remix!! Pop Glow + Mascara Flakes!! Do you like? (Comparison in last pic)</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgtlg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1dgtbj4</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>✨️ 🎀✨️</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgtbj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1dgt9d0</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Polishes like Fair Isle by LynB but warmer?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgt9d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1dgt596</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>To All Who Ghosted Me this summer</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgt596</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1dgsn54</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish Thinner Reccomendation </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgsn54/polish_thinner_reccomendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1dgs8ah</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>essie ballet slipper alternatives (so streaky!)</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgs8ah/essie_ballet_slipper_alternatives_so_streaky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1dgqa31</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Happy Captain Picard Day to all who celebrate!</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/on61tzyfks6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1dgpcy0</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Been awhile since I’ve done a creme-only manicure!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgpcy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1dgorbg</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>KB Shimmer Patch Things Up</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2g57sdk7s6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1dgo939</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>💙🖤🏳️‍🌈Gender Fluid🏳️‍🌈🩷🤍</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgo939</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1dgn9e5</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>I have recently developed an allergy to nail glue, I want to grow my natural nails out but can’t kick this nasty habit.</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgn9e5/i_have_recently_developed_an_allergy_to_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1dgn95e</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Help with Sally Hansen miracle gel</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrxujyi2vr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1dgmq6t</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Cute flower nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgmq6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1dgm8fm</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>I’m in love</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m7bs2sgmr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1dgm6j7</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>My fault for doing outside stuff but 🥲</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu80j1b0mr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1dgm5q5</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Sunset orange/pink shimmer from existing polishes?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgm5q5/sunset_orangepink_shimmer_from_existing_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1dglqp2</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I have been influenced!</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bddyh3mair6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1dglq8f</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Dip flu?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dglq8f/dip_flu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1dglhs5</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Pride Month calls for holo and sparkly nails. I don’t make the rules. 🌈✨</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dglhs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1dglg3x</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>ILNP Midnight Kiss</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dglg3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1dgk27t</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can buy myself flowers </t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sllv4d654r6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1dgk1nk</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>the world's a little blurry</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgk1nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1dgir1v</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Sticky Nail Polish (Solution)</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgir1v/sticky_nail_polish_solution/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1dgi6gj</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So much fun! </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j0qujbynq6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1dghd50</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>My First Cirque: Time Traveler</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dghd50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1dgfund</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>MOONCAT - Am I Everything You Fear?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgfund</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1dgfapa</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Trying to determine if I have a gel allergy, or just need to see a different nail techs, please help!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgfapa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1dgesvr</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Guest List by ILNP</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/15a7hqblnp6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1dgdxw9</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Peely base coat has changed my life!</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dgdxw9/peely_base_coat_has_changed_my_life/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1dh1dms</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amber nails I designed </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q4q86lzmv6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1dh16vf</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>matte magic for your fingertips</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/po4czroikv6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1dgztk8</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>I always do plain nails, but I think other amazing works of my favorite Nail Tech deserve more recognition. Credit to: https://www.instagram.com/lucy_b_nguyen/</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgztk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1dgzdqs</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>For a concert</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgzdqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1dgylrq</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>second attempt at mermaid nails</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgylrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1dgyfvx</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Purple color changing gel with flowers</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgyfvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1dgvrfv</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>ATLA nails!</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u96bf8snxt6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1dgvirr</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Mermaid 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgvirr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1dgvhuz</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Nail glue with NO methacrylate</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j4zpuszut6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1dgukl6</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Powerpuff Girl</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vlgmspj6mt6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1dgukg7</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Summer Fruit Nails 🍉🍋</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgukg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1dgst02</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Watermelon Sugar 🍉</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/5UH07K7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1dgs7fn</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Getting nail art ready for 4th of July! These are airbrush, made custom nail stickers as well!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24lc4dxt0t6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1dgroyl</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Mid-mani Remix! Whatcha Think?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgroyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1dgqrjh</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈Pride nails, take 2- ✨️ Lesbian edition✨️ (much better)</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgqrjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1dgqpwx</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>mermaid nails</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb7tc9k6os6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1dgmuh9</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Criss-cross bow set </t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmhtx0zmrr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1dgmrot</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Gemstone set for my mom!</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgmrot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1dgmq9s</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>💐❤️💐</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hhv1vdlqr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1dgm02m</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Simple mint green set</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1qj5hnikr6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1dgk3s1</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Print love ❤️ Like?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyrysy9k4r6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1dgjieh</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Create this set with me 💅✨</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgjieh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1dgj538</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Issues with my UV fingerless gloves, has anyone had anything similar?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dgj538/issues_with_my_uv_fingerless_gloves_has_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1dgize9</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Inspired by u/kisasame21 and her pastel pink watermelons 🍉🍉🍉</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hefwkis5vq6d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1dgfvf6</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY soft gel </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dgfvf6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>